<commit_message>
Improving snake.py and updating teams.py
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -14,126 +14,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Absentees</t>
   </si>
   <si>
-    <t>AANYA JAIN</t>
-  </si>
-  <si>
-    <t>AARAV DUA</t>
-  </si>
-  <si>
     <t>AAYUSH GUPTA</t>
   </si>
   <si>
-    <t>AKSHITA PURI</t>
-  </si>
-  <si>
-    <t>ANSHIKA</t>
-  </si>
-  <si>
     <t>ARNAV SHARMA</t>
   </si>
   <si>
     <t>AROUSH SETH</t>
   </si>
   <si>
-    <t>ARSHIA KHAUND</t>
-  </si>
-  <si>
-    <t>ARYAN WALIA</t>
-  </si>
-  <si>
-    <t>AVNI AGGARWAL</t>
-  </si>
-  <si>
-    <t>BHAVYA ARORA</t>
-  </si>
-  <si>
     <t>BHAVYA SHARMA</t>
   </si>
   <si>
     <t>DREESHTI KAPOOR</t>
   </si>
   <si>
-    <t>DIPIN PANDEY</t>
-  </si>
-  <si>
-    <t>DEVANSH PANDEYA</t>
-  </si>
-  <si>
-    <t>EKAANSH GABA</t>
-  </si>
-  <si>
-    <t>ISHANI JHA</t>
-  </si>
-  <si>
     <t>IHINA ROY</t>
   </si>
   <si>
     <t>LAKSHAY MALHOTRA</t>
   </si>
   <si>
-    <t>KASHIKA TAYAL</t>
-  </si>
-  <si>
-    <t>JIAH BAJAJ</t>
-  </si>
-  <si>
-    <t>MAHI WADHWA</t>
-  </si>
-  <si>
     <t>PANKAJ</t>
   </si>
   <si>
     <t>PARTH GUPTA</t>
   </si>
   <si>
-    <t>PRATHAM SHARMA</t>
-  </si>
-  <si>
-    <t>RANVEER SOLANKI</t>
-  </si>
-  <si>
-    <t>RENNIE GUPTA</t>
-  </si>
-  <si>
-    <t>RIHIT RAI</t>
-  </si>
-  <si>
-    <t>RISHABH SINGH</t>
-  </si>
-  <si>
-    <t>ROUNAK BISWAS</t>
-  </si>
-  <si>
-    <t>RUDRA VIJ</t>
-  </si>
-  <si>
-    <t>SANYAM MATHUR</t>
-  </si>
-  <si>
-    <t>SASHVI SINGLA</t>
-  </si>
-  <si>
-    <t>SHARVI SINGHAL</t>
-  </si>
-  <si>
     <t>SUMAN</t>
-  </si>
-  <si>
-    <t>UNNABH BHALLA</t>
-  </si>
-  <si>
-    <t>VANSHIKA ARYA</t>
-  </si>
-  <si>
-    <t>YANA VIG</t>
-  </si>
-  <si>
-    <t>YUVRAJ MALIK</t>
   </si>
 </sst>
 </file>
@@ -491,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -582,238 +495,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="1">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="1">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="1">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="1">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="1">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="1">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="1">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="1">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="1">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="1">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
-      <c r="A39" s="1">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>39</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improving my selenium skills now.
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Absentees</t>
   </si>
@@ -25,39 +25,69 @@
     <t>AARAV DUA</t>
   </si>
   <si>
+    <t>AAYUSH GUPTA</t>
+  </si>
+  <si>
     <t>AKSHITA PURI</t>
   </si>
   <si>
+    <t>ANEESH RAMAN</t>
+  </si>
+  <si>
     <t>ANSHIKA</t>
   </si>
   <si>
     <t>ARNAV SHARMA</t>
   </si>
   <si>
+    <t>AROUSH SETH</t>
+  </si>
+  <si>
     <t>ARSHIA KHAUND</t>
   </si>
   <si>
     <t>ARYAN WALIA</t>
   </si>
   <si>
+    <t>AVNI AGGARWAL</t>
+  </si>
+  <si>
+    <t>BHAVYA ARORA</t>
+  </si>
+  <si>
     <t>BHAVYA SHARMA</t>
   </si>
   <si>
+    <t>DREESHTI KAPOOR</t>
+  </si>
+  <si>
     <t>DIPIN PANDEY</t>
   </si>
   <si>
+    <t>DEVANSH PANDEYA</t>
+  </si>
+  <si>
     <t>EKAANSH GABA</t>
   </si>
   <si>
     <t>ISHANI JHA</t>
   </si>
   <si>
+    <t>IHINA ROY</t>
+  </si>
+  <si>
+    <t>LAKSHAY MALHOTRA</t>
+  </si>
+  <si>
     <t>KASHIKA TAYAL</t>
   </si>
   <si>
     <t>JIAH BAJAJ</t>
   </si>
   <si>
+    <t>MAHI WADHWA</t>
+  </si>
+  <si>
     <t>PANKAJ</t>
   </si>
   <si>
@@ -67,6 +97,9 @@
     <t>PRATHAM SHARMA</t>
   </si>
   <si>
+    <t>RANVEER SOLANKI</t>
+  </si>
+  <si>
     <t>RENNIE GUPTA</t>
   </si>
   <si>
@@ -79,6 +112,18 @@
     <t>ROUNAK BISWAS</t>
   </si>
   <si>
+    <t>RUDRA VIJ</t>
+  </si>
+  <si>
+    <t>SANYAM MATHUR</t>
+  </si>
+  <si>
+    <t>SASHVI SINGLA</t>
+  </si>
+  <si>
+    <t>SHARVI SINGHAL</t>
+  </si>
+  <si>
     <t>SUMAN</t>
   </si>
   <si>
@@ -86,6 +131,12 @@
   </si>
   <si>
     <t>VANSHIKA ARYA</t>
+  </si>
+  <si>
+    <t>YANA VIG</t>
+  </si>
+  <si>
+    <t>YUVRAJ MALIK</t>
   </si>
 </sst>
 </file>
@@ -443,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -638,6 +689,142 @@
         <v>23</v>
       </c>
     </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding all the important data
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AAYUSH GUPTA</t>
+          <t>AANYA JAIN</t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ANSHIKA</t>
+          <t>AARAV DUA</t>
         </is>
       </c>
     </row>
@@ -466,7 +466,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BHAVYA SHARMA</t>
+          <t>AAYUSH GUPTA</t>
         </is>
       </c>
     </row>
@@ -476,7 +476,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DIPIN PANDEY</t>
+          <t>AKSHITA PURI</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ISHANI JHA</t>
+          <t>ANSHIKA</t>
         </is>
       </c>
     </row>
@@ -496,7 +496,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>MAHI WADHWA</t>
+          <t>ARNAV SHARMA</t>
         </is>
       </c>
     </row>
@@ -506,7 +506,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>PANKAJ</t>
+          <t>AROUSH SETH</t>
         </is>
       </c>
     </row>
@@ -516,7 +516,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>PARTH GUPTA</t>
+          <t>BHAVYA SHARMA</t>
         </is>
       </c>
     </row>
@@ -526,7 +526,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>PRATHAM SHARMA</t>
+          <t>DIPIN PANDEY</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RENNIE GUPTA</t>
+          <t>ISHANI JHA</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SANYAM MATHUR</t>
+          <t>LAKSHAY MALHOTRA</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SUMAN</t>
+          <t>KASHIKA TAYAL</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>UNNABH BHALLA</t>
+          <t>MAHI WADHWA</t>
         </is>
       </c>
     </row>
@@ -576,7 +576,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>VANSHIKA ARYA</t>
+          <t>PANKAJ</t>
         </is>
       </c>
     </row>
@@ -585,6 +585,76 @@
         <v>15</v>
       </c>
       <c r="B16" t="inlineStr">
+        <is>
+          <t>PRATHAM SHARMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>RANVEER SOLANKI</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>RISHABH SINGH</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ROUNAK BISWAS</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>SUMAN</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>UNNABH BHALLA</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>VANSHIKA ARYA</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>YUVRAJ MALIK</t>
         </is>

</xml_diff>